<commit_message>
Add .gitignore files to avoid pushing useless materials
</commit_message>
<xml_diff>
--- a/report/excelReport/DemoAPITestCase_Isolate.xlsx
+++ b/report/excelReport/DemoAPITestCase_Isolate.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -75,6 +75,11 @@
       <b val="1"/>
       <color rgb="00A52A2A"/>
     </font>
+    <font>
+      <name val="宋体"/>
+      <b val="1"/>
+      <color rgb="00FF0000"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -119,7 +124,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -161,6 +166,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -681,7 +689,7 @@
       </c>
       <c r="N2" s="7" t="inlineStr">
         <is>
-          <t>{'access_token': 'fd8a1748-7391-4be5-9c4b-f673d3cf827f', 'token_type': 'bearer', 'refresh_token': '4a83b2ea-8927-4d66-8585-54478ee221d5', 'expires_in': 16221, 'scope': 'server', 'tenant_id': 'TAX', 'license': 'made by ling', 'eName': 'edmspicMic', 'staffNo': '1002', 'user_id': '9e2f885f-fccc-4f6c-9df7-5f42b421b7db', 'cName': '自动化用户002', 'active': True, 'dept_id': None, 'username': 'autoMic'}</t>
+          <t>{'access_token': 'eeef7aa9-4555-4f1a-be0e-aecb559e1ded', 'token_type': 'bearer', 'refresh_token': '11aeea9c-abdb-4ee5-89c8-35ec6cba9f65', 'expires_in': 31551, 'scope': 'server', 'tenant_id': 'TAX', 'license': 'made by ling', 'eName': 'edmspicMic', 'staffNo': '1002', 'user_id': '9e2f885f-fccc-4f6c-9df7-5f42b421b7db', 'cName': '自动化用户002', 'active': True, 'dept_id': None, 'username': 'autoMic'}</t>
         </is>
       </c>
     </row>
@@ -729,9 +737,9 @@
         </is>
       </c>
       <c r="K3" s="6" t="n"/>
-      <c r="L3" s="13" t="inlineStr">
-        <is>
-          <t>PASS</t>
+      <c r="L3" s="15" t="inlineStr">
+        <is>
+          <t>FAIL</t>
         </is>
       </c>
       <c r="M3" s="14" t="inlineStr">
@@ -741,7 +749,7 @@
       </c>
       <c r="N3" s="7" t="inlineStr">
         <is>
-          <t>{'code': 0, 'message': None, 'data': {'recordCount': 83, 'pageIndex': 1, 'pageSize': 15, 'result': [{'createdBy': '1002', 'createdByEnName': 'edmspicMic', 'createdByName': '自动化用户002', 'createDate': '2021-10-15 09:33:23', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 2, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': '0d4e709b-e468-4774-bdc8-985498595125', 'code': '', 'projectName': 'test', 'clientName': 'cn-name', 'clientCode': '', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '1001', 'riskReviewer': '', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'edmspicStaff', 'riskReviewerName': '', 'fisY': 2022, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': '', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': '', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CON SAM Central', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': '', 'engLetterNo': '', 'serviceOffering': '', 'serviceOfferingDesc': '', 'businessType': '', 'engagementRisk': '', 'projectPeriod': '202108,202110', 'projectPeriodDiff': 3, 'ppic': '', 'ppicName': '', 'archivedRecallStatus': None, 'completenessReviewStatus': 'Not Started', 'codePic': '', 'codePicName': '', 'codeMic': '', 'codeMicName': '', 'masterEngComp': '', 'engCodeCompany': '', 'engagementDesc': '', 'confidentialityRisk': '', 'regionCode': '', 'locationCode': '', 'rcCode': '', 'industryDesc': '', 'industryCode': '', 'toolkitStatus': '未开始', 'isMasterEng': '', 'opportunityId': '', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': None, 'startDate': None, 'closeDate': None, 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '1002', 'createdByEnName': 'edmspicMic', 'createdByName': '自动化用户002', 'createDate': '2021-10-13 16:33:42', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 2, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': 'dc157343-7b6a-4e8e-9134-ff8dd4353990', 'code': '8080-DC453524-HH-02-CON', 'projectName': '流程更改回归测试', 'clientName': 'HuaLongWang-MassiveData HLW CO. LTD', 'clientCode': '8080', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '1001', 'riskReviewer': '', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'edmspicStaff', 'riskReviewerName': '', 'fisY': 2021, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': 'CEA-MU-DC-453524', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': '', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CON SAM STRATEGY', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': 'USD', 'engLetterNo': 'EL19FDC453524', 'serviceOffering': '', 'serviceOfferingDesc': 'SAM M&amp;A', 'businessType': '', 'engagementRisk': 'Much Great', 'projectPeriod': '202108,202110', 'projectPeriodDiff': 3, 'ppic': '10014', 'ppicName': 'edmsmicPpic', 'archivedRecallStatus': None, 'completenessReviewStatus': 'Not Started', 'codePic': '1003', 'codePicName': 'edmspicPic', 'codeMic': '1002', 'codeMicName': 'edmspicMic', 'masterEngComp': 'MU7A', 'engCodeCompany': 'MU7A', 'engagementDesc': 'AutoTest-20210926-152739', 'confidentialityRisk': 'Normal', 'regionCode': 'GDC', 'locationCode': 'MU', 'rcCode': 'MU6618F060', 'industryDesc': 'Consumer/RWD/Specialty and Department Stores', 'industryCode': 'CRS2', 'toolkitStatus': '未开始', 'isMasterEng': 'Y', 'opportunityId': '453524', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': 50000.0, 'startDate': '2021-06-05 00:00:00', 'closeDate': None, 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '1002', 'createdByEnName': 'edmspicMic', 'createdByName': '自动化用户002', 'createDate': '2021-09-27 14:22:39', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 3, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': '1361ded2-ab2d-40a2-8625-c186b09cb630', 'code': '8080-DC453532-HH-02-CON', 'projectName': '检查service line', 'clientName': 'HuaLongWang-MassiveData HLW CO. LTD', 'clientCode': '8080', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '1001', 'riskReviewer': '', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'edmspicStaff', 'riskReviewerName': '', 'fisY': 2021, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': 'CEA-SH-DC-453532', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': '', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CON CENT UCHIDA', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': 'USD', 'engLetterNo': 'EL19FDC453532', 'serviceOffering': '', 'serviceOfferingDesc': 'CBO SCNO', 'businessType': '', 'engagementRisk': 'Much Great', 'projectPeriod': '202108,202109', 'projectPeriodDiff': 2, 'ppic': '10014', 'ppicName': 'edmsmicPpic', 'archivedRecallStatus': None, 'completenessReviewStatus': 'Not Started', 'codePic': '1003', 'codePicName': 'edmspicPic', 'codeMic': '1002', 'codeMicName': 'edmspicMic', 'masterEngComp': 'SH3A', 'engCodeCompany': 'SH3A', 'engagementDesc': 'AutoTest-20210926-152741', 'confidentialityRisk': 'Medium', 'regionCode': 'EC', 'locationCode': 'SH', 'rcCode': 'SH16181040', 'industryDesc': 'ER&amp;I/IP&amp;C/Industrial Products', 'industryCode': 'EIP1', 'toolkitStatus': '未开始', 'isMasterEng': 'Y', 'opportunityId': '453532', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': 50000.0, 'startDate': '2021-06-05 00:00:00', 'closeDate': '2021-10-11 16:09:15', 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '170598', 'createdByEnName': 'Taoism LEE', 'createdByName': '李于', 'createDate': '2021-09-23 10:35:35', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 3, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': 'ca502f51-dabd-4e23-a567-64508b995a42', 'code': '', 'projectName': '检查邮件插件002', 'clientName': '检查邮件插件002-CN', 'clientCode': '', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '170598', 'riskReviewer': '', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'Taoism LEE', 'riskReviewerName': '', 'fisY': 2022, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': '', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': 'true', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CON AP Funding', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': '', 'engLetterNo': '', 'serviceOffering': '', 'serviceOfferingDesc': '', 'businessType': '', 'engagementRisk': '', 'projectPeriod': '202108,202109', 'projectPeriodDiff': 2, 'ppic': '', 'ppicName': '', 'archivedRecallStatus': None, 'completenessReviewStatus': 'Not Started', 'codePic': '', 'codePicName': '', 'codeMic': '', 'codeMicName': '', 'masterEngComp': '', 'engCodeCompany': '', 'engagementDesc': '', 'confidentialityRisk': '', 'regionCode': '', 'locationCode': '', 'rcCode': '', 'industryDesc': '', 'industryCode': '', 'toolkitStatus': '未开始', 'isMasterEng': '', 'opportunityId': '', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': None, 'startDate': None, 'closeDate': None, 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '1002', 'createdByEnName': 'edmspicMic', 'createdByName': '自动化用户002', 'createDate': '2021-09-24 11:07:44', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 2, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': 'ccf1a101-5e3b-44df-b6fe-7659089a30b8', 'code': '', 'projectName': '123', 'clientName': '123', 'clientCode': '', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '1001', 'riskReviewer': '', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'edmspicStaff', 'riskReviewerName': '', 'fisY': 2022, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': '', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': '', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CON Alliance', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': '', 'engLetterNo': '', 'serviceOffering': '', 'serviceOfferingDesc': '', 'businessType': '', 'engagementRisk': '', 'projectPeriod': '202108,202109', 'projectPeriodDiff': 2, 'ppic': '', 'ppicName': '', 'archivedRecallStatus': None, 'completenessReviewStatus': 'Not Started', 'codePic': '', 'codePicName': '', 'codeMic': '', 'codeMicName': '', 'masterEngComp': '', 'engCodeCompany': '', 'engagementDesc': '', 'confidentialityRisk': '', 'regionCode': '', 'locationCode': '', 'rcCode': '', 'industryDesc': '', 'industryCode': '', 'toolkitStatus': '未开始', 'isMasterEng': '', 'opportunityId': '', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': None, 'startDate': None, 'closeDate': None, 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '170598', 'createdByEnName': 'Taoism LEE', 'createdByName': '李于', 'createDate': '2021-09-23 10:34:43', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 2, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': '2babe885-1470-40ea-b697-dcc8aea176f9', 'code': '', 'projectName': '检查邮件插件001', 'clientName': '检查邮件插件001-CN', 'clientCode': '', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '170598', 'riskReviewer': '', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'Taoism LEE', 'riskReviewerName': '', 'fisY': 2022, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': '', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': '', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CON Alliance', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': '', 'engLetterNo': '', 'serviceOffering': '', 'serviceOfferingDesc': '', 'businessType': '', 'engagementRisk': '', 'projectPeriod': '202108,202109', 'projectPeriodDiff': 2, 'ppic': '', 'ppicName': '', 'archivedRecallStatus': None, 'completenessReviewStatus': 'Not Started', 'codePic': '', 'codePicName': '', 'codeMic': '', 'codeMicName': '', 'masterEngComp': '', 'engCodeCompany': '', 'engagementDesc': '', 'confidentialityRisk': '', 'regionCode': '', 'locationCode': '', 'rcCode': '', 'industryDesc': '', 'industryCode': '', 'toolkitStatus': '未开始', 'isMasterEng': '', 'opportunityId': '', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': None, 'startDate': None, 'closeDate': None, 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '1002', 'createdByEnName': 'edmspicMic', 'createdByName': '自动化用户002', 'createDate': '2021-09-10 16:28:32', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 2, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': '7cf392e8-824f-488f-a0dd-ed17d7cf342a', 'code': '', 'projectName': 'quals导出2', 'clientName': 'quals导出2-CN', 'clientCode': '', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '1001', 'riskReviewer': '1005', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'edmspicStaff', 'riskReviewerName': 'edmspicSpecialRisk', 'fisY': 2022, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': '', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': '', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CON Alliance', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': '', 'engLetterNo': '', 'serviceOffering': '', 'serviceOfferingDesc': '', 'businessType': '', 'engagementRisk': '', 'projectPeriod': '202108,202109', 'projectPeriodDiff': 2, 'ppic': '10014', 'ppicName': 'edmsmicPpic', 'archivedRecallStatus': None, 'completenessReviewStatus': 'Not Started', 'codePic': '', 'codePicName': '', 'codeMic': '', 'codeMicName': '', 'masterEngComp': '', 'engCodeCompany': '', 'engagementDesc': '', 'confidentialityRisk': '', 'regionCode': '', 'locationCode': '', 'rcCode': '', 'industryDesc': '', 'industryCode': '', 'toolkitStatus': '未开始', 'isMasterEng': '', 'opportunityId': '', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': None, 'startDate': None, 'closeDate': None, 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '1002', 'createdByEnName': 'edmspicMic', 'createdByName': '自动化用户002', 'createDate': '2021-09-10 15:56:51', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 2, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': 'da02a8d9-a0db-430c-9ac4-db05c9d20ef6', 'code': '8080-DC453122-HH-02-CON', 'projectName': 'quals导出', 'clientName': 'HuaLongWang-MassiveData HLW CO. LTD', 'clientCode': '8080', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '1001', 'riskReviewer': '1005', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'edmspicStaff', 'riskReviewerName': 'edmspicSpecialRisk', 'fisY': 2021, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': 'CEA-BJ-DC-453122', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': '', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CON C&amp;M Digital Customer', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': '', 'engLetterNo': 'EL19FDC453122', 'serviceOffering': '', 'serviceOfferingDesc': 'SAM Central', 'businessType': '', 'engagementRisk': '', 'projectPeriod': '202108,202109', 'projectPeriodDiff': 2, 'ppic': '10014', 'ppicName': 'edmsmicPpic', 'archivedRecallStatus': None, 'completenessReviewStatus': 'Not Started', 'codePic': '', 'codePicName': '', 'codeMic': '', 'codeMicName': '', 'masterEngComp': '', 'engCodeCompany': '', 'engagementDesc': '', 'confidentialityRisk': '', 'regionCode': '', 'locationCode': '', 'rcCode': '', 'industryDesc': '', 'industryCode': '', 'toolkitStatus': '未开始', 'isMasterEng': '', 'opportunityId': '', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': None, 'startDate': None, 'closeDate': None, 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '1002', 'createdByEnName': 'edmspicMic', 'createdByName': '自动化用户002', 'createDate': '2021-09-10 10:05:01', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Completed', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 6, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': '21511ebc-2dd7-4670-9bea-4590232cab92', 'code': '8080-DC453123-HH-02-CON', 'projectName': '按钮权限验证', 'clientName': 'HuaLongWang-MassiveData HLW CO. LTD', 'clientCode': '8080', 'isRecord': True, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '1001', 'riskReviewer': '1005', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'edmspicStaff', 'riskReviewerName': 'edmspicSpecialRisk', 'fisY': 2021, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': 'CEA-SH-DC-453123', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': '', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CON AP Funding', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': '', 'engLetterNo': 'EL19FDC453123', 'serviceOffering': '', 'serviceOfferingDesc': 'SAM Strategy', 'businessType': '', 'engagementRisk': '', 'projectPeriod': '202107,202108', 'projectPeriodDiff': 2, 'ppic': '10014', 'ppicName': 'edmsmicPpic', 'archivedRecallStatus': False, 'completenessReviewStatus': 'Completed', 'codePic': '', 'codePicName': '', 'codeMic': '', 'codeMicName': '', 'masterEngComp': '', 'engCodeCompany': '', 'engagementDesc': '', 'confidentialityRisk': '', 'regionCode': '', 'locationCode': '', 'rcCode': '', 'industryDesc': '', 'industryCode': '', 'toolkitStatus': '审核完成', 'isMasterEng': '', 'opportunityId': '', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': None, 'startDate': None, 'closeDate': None, 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '1002', 'createdByEnName': 'edmspicMic', 'createdByName': '自动化用户002', 'createDate': '2021-09-09 15:03:15', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 16, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': '9c7cdda6-076f-4da8-930c-085739e4ebc0', 'code': '8080-DC452890-HH-02-CON', 'projectName': '检查邮件模板中service line均已修改2', 'clientName': 'HuaLongWang-MassiveData HLW CO. LTD', 'clientCode': '8080', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '1001', 'riskReviewer': '', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'edmspicStaff', 'riskReviewerName': '', 'fisY': 2021, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': 'CEA-SH-DC-452890', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': 'true', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CON C&amp;M Digital Customer', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': 'USD', 'engLetterNo': 'EL19FDC452890', 'serviceOffering': 'OAC', 'serviceOfferingDesc': 'SAM Analytics &amp; Cognitive', 'businessType': '', 'engagementRisk': '', 'projectPeriod': '202107,202108', 'projectPeriodDiff': 2, 'ppic': '1004', 'ppicName': 'edmspicCpic', 'archivedRecallStatus': True, 'completenessReviewStatus': 'Not Started', 'codePic': '', 'codePicName': '', 'codeMic': '', 'codeMicName': '', 'masterEngComp': '', 'engCodeCompany': '', 'engagementDesc': '', 'confidentialityRisk': '', 'regionCode': '', 'locationCode': '', 'rcCode': '', 'industryDesc': '', 'industryCode': '', 'toolkitStatus': '退回', 'isMasterEng': '', 'opportunityId': '', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': None, 'startDate': None, 'closeDate': None, 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '1002', 'createdByEnName': 'edmspicMic', 'createdByName': '自动化用户002', 'createDate': '2021-09-09 14:12:21', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 10, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': 'f03ae401-c93d-4036-a830-e7e5b77945ee', 'code': '8080-DC452932-HH-02-CON', 'projectName': '检查邮件模板中service line均已修改', 'clientName': 'HuaLongWang-MassiveData HLW CO. LTD', 'clientCode': '8080', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '1001', 'riskReviewer': '', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'edmspicStaff', 'riskReviewerName': '', 'fisY': 2021, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': 'CEA-SH-DC-452932', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': '', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CON C&amp;M Digital Customer', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': 'USD', 'engLetterNo': 'EL19FDC452932', 'serviceOffering': 'OAT', 'serviceOfferingDesc': 'HC Actuarial', 'businessType': '', 'engagementRisk': '', 'projectPeriod': '202107,202108', 'projectPeriodDiff': 2, 'ppic': '1003', 'ppicName': 'edmspic003452413', 'archivedRecallStatus': None, 'completenessReviewStatus': 'Reviewing', 'codePic': '', 'codePicName': '', 'codeMic': '', 'codeMicName': '', 'masterEngComp': '', 'engCodeCompany': '', 'engagementDesc': '', 'confidentialityRisk': '', 'regionCode': '', 'locationCode': '', 'rcCode': '', 'industryDesc': '', 'industryCode': '', 'toolkitStatus': '待KM Toolkit Reviewer审核', 'isMasterEng': '', 'opportunityId': '', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': None, 'startDate': None, 'closeDate': None, 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '1002', 'createdByEnName': 'edmspicMic', 'createdByName': '自动化用户002', 'createDate': '2021-09-08 17:27:36', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 2, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': '23875bed-6bc5-4756-8df6-978937d09604', 'code': '8080-DC452931-HH-02-CON', 'projectName': 'catalog查询条件优化', 'clientName': 'HuaLongWang-MassiveData HLW CO. LTD', 'clientCode': '8080', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '1001', 'riskReviewer': '', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'edmspicStaff', 'riskReviewerName': '', 'fisY': 2021, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': 'CEA-BJ-DC-452931', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': '', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'SAM-Strategy', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': '', 'engLetterNo': 'EL19FDC452931', 'serviceOffering': 'OAT', 'serviceOfferingDesc': 'HC Actuarial', 'businessType': '', 'engagementRisk': '', 'projectPeriod': '202108,202109', 'projectPeriodDiff': 2, 'ppic': '1003', 'ppicName': 'edmspicPic', 'archivedRecallStatus': None, 'completenessReviewStatus': 'Not Started', 'codePic': '', 'codePicName': '', 'codeMic': '', 'codeMicName': '', 'masterEngComp': '', 'engCodeCompany': '', 'engagementDesc': '', 'confidentialityRisk': '', 'regionCode': '', 'locationCode': '', 'rcCode': '', 'industryDesc': '', 'industryCode': '', 'toolkitStatus': '未开始', 'isMasterEng': '', 'opportunityId': '', 'targetCountryCode': '', 'restrictionOnDisclosure': '', 'summaryOfEngagement': '', 'estFee': None, 'startDate': None, 'closeDate': None, 'associatedCode': None, 'masterCompanyCode': None, 'alliancePartner': '', 'alliancePartnerDesc': '', 'masterEngCode': '', 'forceDelete': True, 'log': False}, {'createdBy': '1002', 'createdByEnName': 'edmspicMic', 'createdByName': '自动化用户002', 'createDate': '2021-09-08 16:59:39', 'modifiedBy': None, 'modifiedByEnName': None, 'modifiedByName': None, 'modifiedDate': None, 'status': 'Ongoing', 'operationOrgCode': None, 'dataOwner': None, 'tenantId': None, 'archiveBaseDate': None, 'versionId': 2, 'delFlag': '0', 'deleteBy': None, 'deleteDate': None, 'subSystem': None, 'id': '17f6507e-d3a2-4e77-bb22-f283df871b99', 'code': '8080-DC453044-HH-02-CON', 'projectName': '检查desc及查询', 'clientName': 'HuaLongWang2-MassiveData HLW CO. LTD', 'clientCode': '8080', 'isRecord': False, 'archiveDuration': '10', 'archiveNo': '', 'archiveCommitor': '', 'archiveCommitorNo': '', 'archiveCommitDate': None, 'archiveMailDate': None, 'archiveReviewer': None, 'pic': '1003', 'mic': '1002', 'aic': '', 'staff': '1001', 'riskReviewer': '', 'picName': 'edmspicPic', 'micName': 'edmspicMic', 'aicName': '', 'staffName': 'edmspicStaff', 'riskReviewerName': '', 'fisY': 2021, 'sourceFrom': None, 'proStatus': 1, 'spic': '', 'spicName': '', 'conPartner': '1004', 'conPartnerName': 'edmspicCpic', 'bark': '', 'isShare': None, 'proInsId': '', 'projectType': 'Implementation', 'finalReviewRole': '', 'finalReviewer': '', 'finalReviewerName': '', 'ceaNo': 'CEA-SH-DC-453044', 'noCeaReason': '', 'qrmTrace': '', 'kmTrace': '', 'lastWithdrawAuditCompletedDate': None, 'serviceLine': 'CIM', 'toolkitTemplate': '589C9511-5526-43CB-872A-C72C81F3C948', 'toolkitTemplateName': 'Toolkit  General', 'toolkitRemark': 'Toolkit  General', 'fileCatalogTemplateId': '712C340B-074C-43C6-9F9A-9987B6D9BC76', 'createRootFolder': False, 'contractCurrency': '', 'engLetterNo': 'EL19FDC453</t>
+          <t>{'code': 40025003, 'message': 'Token不存在或验证错误', 'data': '8b0dc6ca-71d1-4581-9942-4c30b16ce49d', 'success': False, 'msg': 'Token不存在或验证错误'}</t>
         </is>
       </c>
     </row>

</xml_diff>